<commit_message>
Reviewer 2 modify suppt4
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_4_monthly_deaths.xlsx
+++ b/Figures_Tables/Supp_Table_4_monthly_deaths.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Age group</t>
   </si>
@@ -20,37 +20,144 @@
     <t xml:space="preserve">Year-Month</t>
   </si>
   <si>
-    <t xml:space="preserve">Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-11</t>
+    <t xml:space="preserve">Non vaccinated deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccinated deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-2 years old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-11 years old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-17 years old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,9 +180,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,389 +485,497 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>43891</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>43922</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>43952</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>43983</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>44013</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>44044</v>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>44075</v>
-      </c>
-      <c r="C8" t="n">
-        <v>12</v>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>44105</v>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>44136</v>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>44166</v>
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>44197</v>
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>44228</v>
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>44256</v>
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>44287</v>
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="n">
         <v>3</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>44317</v>
-      </c>
-      <c r="C16" t="n">
-        <v>10</v>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>44348</v>
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>44378</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
       </c>
       <c r="C18" t="n">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>44409</v>
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
       </c>
       <c r="C19" t="n">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>44440</v>
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
       </c>
       <c r="C20" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>44470</v>
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>44501</v>
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>44531</v>
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
       </c>
       <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>44562</v>
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
       </c>
       <c r="C24" t="n">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>44593</v>
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
       </c>
       <c r="C25" t="n">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>44621</v>
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>44652</v>
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
       </c>
       <c r="C27" t="n">
+        <v>11</v>
+      </c>
+      <c r="D27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>44682</v>
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
       </c>
       <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>44713</v>
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>44743</v>
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>44774</v>
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>44805</v>
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
       </c>
       <c r="C32" t="n">
         <v>2</v>
       </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="n">
         <v>3</v>
       </c>
-      <c r="B33" s="1" t="n">
-        <v>44835</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1</v>
+      <c r="D33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>44866</v>
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>44896</v>
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="n">
-        <v>43891</v>
+      <c r="B36" t="s">
+        <v>39</v>
       </c>
       <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -769,736 +983,1035 @@
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1" t="n">
-        <v>43922</v>
+      <c r="B37" t="s">
+        <v>40</v>
       </c>
       <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>43952</v>
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1" t="n">
-        <v>43983</v>
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <v>44013</v>
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <v>44044</v>
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="n">
-        <v>44075</v>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <v>44105</v>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>44136</v>
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
       </c>
       <c r="C44" t="n">
         <v>4</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1" t="n">
-        <v>44166</v>
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="1" t="n">
-        <v>44197</v>
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>44228</v>
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
       </c>
       <c r="C47" t="n">
         <v>4</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <v>44256</v>
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
       </c>
       <c r="C48" t="n">
         <v>4</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>44287</v>
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
       </c>
       <c r="C49" t="n">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>4</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <v>44317</v>
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
       </c>
       <c r="C50" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="1" t="n">
-        <v>44348</v>
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
       </c>
       <c r="C51" t="n">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1" t="n">
-        <v>44378</v>
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
       </c>
       <c r="C52" t="n">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="1" t="n">
-        <v>44409</v>
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
       </c>
       <c r="C53" t="n">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="1" t="n">
-        <v>44440</v>
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
       </c>
       <c r="C54" t="n">
+        <v>9</v>
+      </c>
+      <c r="D54" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="1" t="n">
-        <v>44470</v>
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <v>44501</v>
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
       </c>
       <c r="C56" t="n">
+        <v>7</v>
+      </c>
+      <c r="D56" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <v>44531</v>
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
       </c>
       <c r="C57" t="n">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="1" t="n">
-        <v>44562</v>
+        <v>41</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
       </c>
       <c r="C58" t="n">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="1" t="n">
-        <v>44593</v>
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
       </c>
       <c r="C59" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>44621</v>
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
       </c>
       <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="1" t="n">
-        <v>44652</v>
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
       </c>
       <c r="C61" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>44682</v>
+        <v>41</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>44713</v>
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>30</v>
       </c>
       <c r="C63" t="n">
         <v>3</v>
       </c>
+      <c r="D63" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>44743</v>
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>31</v>
       </c>
       <c r="C64" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="1" t="n">
-        <v>44774</v>
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="1" t="n">
-        <v>44805</v>
+        <v>41</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
       </c>
       <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" s="1" t="n">
-        <v>44835</v>
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>34</v>
       </c>
       <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" s="1" t="n">
-        <v>44866</v>
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>35</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" s="1" t="n">
-        <v>44896</v>
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>36</v>
       </c>
       <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70" s="1" t="n">
-        <v>43891</v>
+        <v>41</v>
+      </c>
+      <c r="B70" t="s">
+        <v>37</v>
       </c>
       <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" s="1" t="n">
-        <v>43922</v>
+        <v>41</v>
+      </c>
+      <c r="B71" t="s">
+        <v>38</v>
       </c>
       <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="1" t="n">
-        <v>43952</v>
+        <v>41</v>
+      </c>
+      <c r="B72" t="s">
+        <v>39</v>
       </c>
       <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="1" t="n">
-        <v>43983</v>
+        <v>41</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
       </c>
       <c r="C73" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="1" t="n">
-        <v>44013</v>
-      </c>
       <c r="C74" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" s="1" t="n">
-        <v>44044</v>
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
       </c>
       <c r="C75" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B76" s="1" t="n">
-        <v>44075</v>
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
       </c>
       <c r="C76" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77" s="1" t="n">
-        <v>44105</v>
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
       </c>
       <c r="C77" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" s="1" t="n">
-        <v>44136</v>
+        <v>42</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
       </c>
       <c r="C78" t="n">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79" s="1" t="n">
-        <v>44166</v>
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" t="n">
         <v>5</v>
       </c>
-      <c r="B80" s="1" t="n">
-        <v>44197</v>
-      </c>
-      <c r="C80" t="n">
+      <c r="D80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="1" t="n">
-        <v>44228</v>
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
       </c>
       <c r="C81" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" s="1" t="n">
-        <v>44256</v>
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
       </c>
       <c r="C82" t="n">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" t="n">
         <v>5</v>
       </c>
-      <c r="B83" s="1" t="n">
-        <v>44287</v>
-      </c>
-      <c r="C83" t="n">
-        <v>2</v>
+      <c r="D83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="1" t="n">
-        <v>44317</v>
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
       </c>
       <c r="C84" t="n">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85" s="1" t="n">
-        <v>44348</v>
+        <v>42</v>
+      </c>
+      <c r="B85" t="s">
+        <v>16</v>
       </c>
       <c r="C85" t="n">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" s="1" t="n">
-        <v>44378</v>
+        <v>42</v>
+      </c>
+      <c r="B86" t="s">
+        <v>17</v>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="1" t="n">
-        <v>44409</v>
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
       </c>
       <c r="C87" t="n">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="1" t="n">
-        <v>44440</v>
+        <v>42</v>
+      </c>
+      <c r="B88" t="s">
+        <v>19</v>
       </c>
       <c r="C88" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="n">
         <v>5</v>
       </c>
-      <c r="B89" s="1" t="n">
-        <v>44470</v>
-      </c>
-      <c r="C89" t="n">
+      <c r="D89" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90" s="1" t="n">
-        <v>44501</v>
+        <v>42</v>
+      </c>
+      <c r="B90" t="s">
+        <v>21</v>
       </c>
       <c r="C90" t="n">
+        <v>9</v>
+      </c>
+      <c r="D90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91" s="1" t="n">
-        <v>44531</v>
+        <v>42</v>
+      </c>
+      <c r="B91" t="s">
+        <v>22</v>
       </c>
       <c r="C91" t="n">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92" s="1" t="n">
-        <v>44562</v>
+        <v>42</v>
+      </c>
+      <c r="B92" t="s">
+        <v>23</v>
       </c>
       <c r="C92" t="n">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" s="1" t="n">
-        <v>44593</v>
+        <v>42</v>
+      </c>
+      <c r="B93" t="s">
+        <v>24</v>
       </c>
       <c r="C93" t="n">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94" s="1" t="n">
-        <v>44621</v>
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
       </c>
       <c r="C94" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95" s="1" t="n">
-        <v>44652</v>
+        <v>42</v>
+      </c>
+      <c r="B95" t="s">
+        <v>26</v>
       </c>
       <c r="C95" t="n">
         <v>2</v>
       </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="1" t="n">
-        <v>44682</v>
+        <v>42</v>
+      </c>
+      <c r="B96" t="s">
+        <v>27</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97" s="1" t="n">
-        <v>44713</v>
+        <v>42</v>
+      </c>
+      <c r="B97" t="s">
+        <v>28</v>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>5</v>
-      </c>
-      <c r="B98" s="1" t="n">
-        <v>44743</v>
+        <v>42</v>
+      </c>
+      <c r="B98" t="s">
+        <v>29</v>
       </c>
       <c r="C98" t="n">
+        <v>14</v>
+      </c>
+      <c r="D98" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>5</v>
-      </c>
-      <c r="B99" s="1" t="n">
-        <v>44774</v>
+        <v>42</v>
+      </c>
+      <c r="B99" t="s">
+        <v>30</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D99" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>5</v>
-      </c>
-      <c r="B100" s="1" t="n">
-        <v>44805</v>
+        <v>42</v>
+      </c>
+      <c r="B100" t="s">
+        <v>31</v>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>5</v>
-      </c>
-      <c r="B101" s="1" t="n">
-        <v>44835</v>
+        <v>42</v>
+      </c>
+      <c r="B101" t="s">
+        <v>32</v>
       </c>
       <c r="C101" t="n">
+        <v>2</v>
+      </c>
+      <c r="D101" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>5</v>
-      </c>
-      <c r="B102" s="1" t="n">
-        <v>44866</v>
+        <v>42</v>
+      </c>
+      <c r="B102" t="s">
+        <v>33</v>
       </c>
       <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="1" t="n">
-        <v>44896</v>
+        <v>42</v>
+      </c>
+      <c r="B103" t="s">
+        <v>34</v>
       </c>
       <c r="C103" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" t="n">
+        <v>3</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>42</v>
+      </c>
+      <c r="B105" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" t="n">
+        <v>2</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>42</v>
+      </c>
+      <c r="B108" t="s">
+        <v>39</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>42</v>
+      </c>
+      <c r="B109" t="s">
+        <v>40</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>